<commit_message>
Latest Changes On QA
</commit_message>
<xml_diff>
--- a/data/BppTrend/Valid_Import_Files/BOE Equipment Index Factors and Percent Good Factors 2020.xlsx
+++ b/data/BppTrend/Valid_Import_Files/BOE Equipment Index Factors and Percent Good Factors 2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="928" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Document Details" sheetId="7" r:id="rId1"/>
@@ -744,7 +744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <sheetData>
@@ -1088,6 +1090,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13">
       <c r="A1" s="11" t="s">
@@ -3111,7 +3116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7265625" defaultRowHeight="12.5"/>
   <cols>

</xml_diff>